<commit_message>
updated output images and tables
</commit_message>
<xml_diff>
--- a/Tables/tables/T1_algo_benchmark.xlsx
+++ b/Tables/tables/T1_algo_benchmark.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alberic/Desktop/Pro/RouskinLab/papers/Main_Paper/DL_paper_figures/Tables/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{852C626A-DC63-A641-A450-2039DB931440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED87B607-F7F8-AC4D-9C93-E6FEE6C1BA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -130,78 +130,72 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF2CB17E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF25AB82"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4CC26C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF67CC5C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF58C765"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF20928C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1FA088"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF1F988B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB8DE29"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF37B878"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF2AB07F"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF24AA83"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF4CC26C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF67CC5C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF58C765"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF20928C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF1FA088"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF1F988B"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB8DE29"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC8E020"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF25AB82"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF35B779"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF69CD5B"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -227,6 +221,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF20938C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCDE11D"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -390,7 +390,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -443,7 +443,7 @@
     <xf numFmtId="2" fontId="2" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -452,19 +452,16 @@
     <xf numFmtId="2" fontId="3" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="20" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -873,14 +870,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" zoomScale="179" workbookViewId="0">
+      <selection activeCell="M8" sqref="A1:M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="13" width="7.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="2" max="13" width="7.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -957,22 +954,22 @@
         <v>9</v>
       </c>
       <c r="B4" s="3">
-        <v>0.89864795756036953</v>
+        <v>0.90033578311248808</v>
       </c>
       <c r="C4" s="4">
-        <v>0.91057332873344421</v>
+        <v>0.91219185501934807</v>
       </c>
       <c r="D4" s="5">
-        <v>0.89011178559131832</v>
+        <v>0.89170967726640293</v>
       </c>
       <c r="E4" s="6">
-        <v>0.54643776839616676</v>
+        <v>0.54852504470393904</v>
       </c>
       <c r="F4" s="7">
-        <v>0.59998892168499696</v>
+        <v>0.60238973867973789</v>
       </c>
       <c r="G4" s="8">
-        <v>0.56946356530672892</v>
+        <v>0.57163130969627141</v>
       </c>
       <c r="H4" s="9">
         <v>0.68732124809175732</v>
@@ -998,39 +995,39 @@
         <v>10</v>
       </c>
       <c r="B5" s="15">
-        <v>0.88279485605699193</v>
-      </c>
-      <c r="C5" s="16">
-        <v>0.90942988346162701</v>
+        <v>0.88396778766055284</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.91054306778757055</v>
       </c>
       <c r="D5" s="15">
-        <v>0.88034272947338188</v>
-      </c>
-      <c r="E5" s="17">
-        <v>0.57157776482441802</v>
-      </c>
-      <c r="F5" s="18">
-        <v>0.63397453057207109</v>
-      </c>
-      <c r="G5" s="7">
-        <v>0.59834372230554767</v>
-      </c>
-      <c r="H5" s="19">
+        <v>0.88143112399208712</v>
+      </c>
+      <c r="E5" s="8">
+        <v>0.57343671028212106</v>
+      </c>
+      <c r="F5" s="16">
+        <v>0.63623920546659773</v>
+      </c>
+      <c r="G5" s="17">
+        <v>0.60031536271082631</v>
+      </c>
+      <c r="H5" s="18">
         <v>0.75019159838557248</v>
       </c>
-      <c r="I5" s="20">
+      <c r="I5" s="19">
         <v>0.80546265169978137</v>
       </c>
-      <c r="J5" s="21">
+      <c r="J5" s="20">
         <v>0.77446813881397247</v>
       </c>
-      <c r="K5" s="22">
+      <c r="K5" s="21">
         <v>0.44997431586186087</v>
       </c>
-      <c r="L5" s="23">
+      <c r="L5" s="22">
         <v>0.46677677929401401</v>
       </c>
-      <c r="M5" s="24">
+      <c r="M5" s="23">
         <v>0.45658219158649438</v>
       </c>
     </row>
@@ -1038,40 +1035,40 @@
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="25">
-        <v>0.91357781937424565</v>
-      </c>
-      <c r="C6" s="26">
-        <v>0.92769685661655732</v>
-      </c>
-      <c r="D6" s="27">
-        <v>0.90393172698409374</v>
-      </c>
-      <c r="E6" s="28">
-        <v>0.728945273422133</v>
-      </c>
-      <c r="F6" s="29">
-        <v>0.76176731848351598</v>
-      </c>
-      <c r="G6" s="30">
-        <v>0.74136501772201324</v>
-      </c>
-      <c r="H6" s="31">
+      <c r="B6" s="24">
+        <v>0.91454696874160546</v>
+      </c>
+      <c r="C6" s="25">
+        <v>0.92861180776134344</v>
+      </c>
+      <c r="D6" s="26">
+        <v>0.90481692594541629</v>
+      </c>
+      <c r="E6" s="27">
+        <v>0.72762461304753068</v>
+      </c>
+      <c r="F6" s="28">
+        <v>0.76021576209953334</v>
+      </c>
+      <c r="G6" s="29">
+        <v>0.73983789183398385</v>
+      </c>
+      <c r="H6" s="30">
         <v>0.70266992896795277</v>
       </c>
-      <c r="I6" s="32">
+      <c r="I6" s="31">
         <v>0.72044730912894006</v>
       </c>
-      <c r="J6" s="33">
+      <c r="J6" s="32">
         <v>0.70951867140829561</v>
       </c>
-      <c r="K6" s="34">
+      <c r="K6" s="33">
         <v>0.41006922970215481</v>
       </c>
-      <c r="L6" s="35">
+      <c r="L6" s="34">
         <v>0.42918933120866609</v>
       </c>
-      <c r="M6" s="36">
+      <c r="M6" s="35">
         <v>0.41859080232679852</v>
       </c>
     </row>
@@ -1079,40 +1076,40 @@
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="37">
-        <v>0.80926631012059358</v>
-      </c>
-      <c r="C7" s="38">
-        <v>0.96284046594348471</v>
-      </c>
-      <c r="D7" s="39">
-        <v>0.86812032427574171</v>
-      </c>
-      <c r="E7" s="40">
-        <v>0.82445320335997119</v>
-      </c>
-      <c r="F7" s="41">
-        <v>0.88421792099713181</v>
-      </c>
-      <c r="G7" s="42">
-        <v>0.84994587030946867</v>
-      </c>
-      <c r="H7" s="43">
+      <c r="B7" s="36">
+        <v>0.81025983207467678</v>
+      </c>
+      <c r="C7" s="37">
+        <v>0.96503088658346847</v>
+      </c>
+      <c r="D7" s="38">
+        <v>0.86977506958056183</v>
+      </c>
+      <c r="E7" s="39">
+        <v>0.82521732203509712</v>
+      </c>
+      <c r="F7" s="40">
+        <v>0.88659418214217689</v>
+      </c>
+      <c r="G7" s="41">
+        <v>0.85151540817519822</v>
+      </c>
+      <c r="H7" s="42">
         <v>0.57792022526264186</v>
       </c>
-      <c r="I7" s="44">
+      <c r="I7" s="43">
         <v>0.58739823177456851</v>
       </c>
-      <c r="J7" s="43">
+      <c r="J7" s="42">
         <v>0.57862800024449823</v>
       </c>
-      <c r="K7" s="45">
+      <c r="K7" s="44">
         <v>0.21894082086610381</v>
       </c>
-      <c r="L7" s="46">
+      <c r="L7" s="45">
         <v>0.14386106443513799</v>
       </c>
-      <c r="M7" s="47">
+      <c r="M7" s="46">
         <v>0.16299531469121581</v>
       </c>
     </row>

</xml_diff>